<commit_message>
Update Tests 31 and 32
</commit_message>
<xml_diff>
--- a/data/qa/QTP/Test031.xlsx
+++ b/data/qa/QTP/Test031.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="2205" windowWidth="21615" windowHeight="11685"/>
+    <workbookView xWindow="1155" yWindow="2205" windowWidth="19320" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="TST001" sheetId="1" r:id="rId1"/>
@@ -210,19 +210,19 @@
     <t>Study Name=Test031 {timestamp}, Study Description=Test Agilent CN DNACopy Supp</t>
   </si>
   <si>
-    <t>Input data from https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Genomic/Supplemental/caArray_data_source.xls and click save</t>
-  </si>
-  <si>
     <t>Under Genomic Data Sources section, look for row with Experiment Identifier of "EXP-481"; and wait for Status="Not Mapped"</t>
   </si>
   <si>
-    <t>Input Data from https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Genomic/Supplemental/caArray_data_source.xls and click Save Segmentation Data Calculation Configuration</t>
-  </si>
-  <si>
     <t>Under Genomic Data Sources section, look for row with Experiment Identifier of "EXP-481"; and wait for Status="Ready to be loaded"</t>
   </si>
   <si>
     <t>Look for row with Study Name=Test031 {timestamp}</t>
+  </si>
+  <si>
+    <t>Input data from https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Genomic/Supplemental/caArray_data_source_3samples.xls and click save</t>
+  </si>
+  <si>
+    <t>Input Data from https://ncisvn.nci.nih.gov/svn/caintegrator2/trunk/data/qa/Studies/Netherlands_Cairo/Genomic/Supplemental/caArray_data_source_3samples.xls and click Save Segmentation Data Calculation Configuration</t>
   </si>
 </sst>
 </file>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -813,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H16" t="s">
         <v>30</v>
@@ -824,7 +824,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
         <v>53</v>
@@ -846,7 +846,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H19" t="s">
         <v>30</v>
@@ -860,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H20" t="s">
         <v>54</v>
@@ -882,7 +882,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
         <v>42</v>

</xml_diff>